<commit_message>
Added more interview questions and example for init and destroy methods
</commit_message>
<xml_diff>
--- a/src/main/java/com/spring/practice/interview/InterviewQuestions(Spring).xlsx
+++ b/src/main/java/com/spring/practice/interview/InterviewQuestions(Spring).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Questions</t>
   </si>
@@ -172,6 +172,33 @@
   </si>
   <si>
     <t>What is joint point?</t>
+  </si>
+  <si>
+    <t>What is InitializingBean and DisposableBean?</t>
+  </si>
+  <si>
+    <t>What is @Autowired annotation?</t>
+  </si>
+  <si>
+    <t>What are different types of Spring Bean autowiring?</t>
+  </si>
+  <si>
+    <t>byName, byType and byConstructor</t>
+  </si>
+  <si>
+    <t>What’s the difference between @Component, @Controller, @Repository &amp; @Service annotations in Spring?</t>
+  </si>
+  <si>
+    <t>https://javarevisited.blogspot.com/2017/11/difference-between-component-service.html</t>
+  </si>
+  <si>
+    <t>What is PersistenceExceptionTranslationPostProcessor ?</t>
+  </si>
+  <si>
+    <t>How does componenet scanning works in spring?</t>
+  </si>
+  <si>
+    <t>What is @ComponentScan?</t>
   </si>
 </sst>
 </file>
@@ -564,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -731,6 +758,50 @@
     <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="30">
+      <c r="A25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -747,9 +818,11 @@
     <hyperlink ref="B13" r:id="rId7"/>
     <hyperlink ref="B14" r:id="rId8" location="beans-factory-scopes"/>
     <hyperlink ref="B18" r:id="rId9"/>
+    <hyperlink ref="B25" r:id="rId10"/>
+    <hyperlink ref="B27" r:id="rId11"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
new example added for nested bean
</commit_message>
<xml_diff>
--- a/src/main/java/com/spring/practice/interview/InterviewQuestions(Spring).xlsx
+++ b/src/main/java/com/spring/practice/interview/InterviewQuestions(Spring).xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Questions</t>
   </si>
@@ -199,6 +199,27 @@
   </si>
   <si>
     <t>What is @ComponentScan?</t>
+  </si>
+  <si>
+    <t>How spring framework works?</t>
+  </si>
+  <si>
+    <t>https://javarevisited.blogspot.com/2017/06/how-spring-mvc-framework-works-web-flow.html</t>
+  </si>
+  <si>
+    <t>Why do we use ApplicationContext over BeanFactory?</t>
+  </si>
+  <si>
+    <t>https://dzone.com/articles/difference-between-beanfactory-and-applicationcont</t>
+  </si>
+  <si>
+    <t>https://howtodoinjava.com/spring-core/spring-bean-post-processors/</t>
+  </si>
+  <si>
+    <t>What is BeanPostProcessor?</t>
+  </si>
+  <si>
+    <t>What is BeanFactoryPostProcessor?</t>
   </si>
 </sst>
 </file>
@@ -591,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -802,6 +823,35 @@
     <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -820,9 +870,12 @@
     <hyperlink ref="B18" r:id="rId9"/>
     <hyperlink ref="B25" r:id="rId10"/>
     <hyperlink ref="B27" r:id="rId11"/>
+    <hyperlink ref="B29" r:id="rId12"/>
+    <hyperlink ref="B30" r:id="rId13"/>
+    <hyperlink ref="B31" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId15"/>
 </worksheet>
 </file>
 

</xml_diff>